<commit_message>
spreadsheet update w php
</commit_message>
<xml_diff>
--- a/supporing_docs/script_tracker.xlsx
+++ b/supporing_docs/script_tracker.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="65">
   <si>
     <t>Output</t>
   </si>
@@ -205,6 +205,15 @@
   </si>
   <si>
     <t>csh</t>
+  </si>
+  <si>
+    <t>select w pattern</t>
+  </si>
+  <si>
+    <t>global</t>
+  </si>
+  <si>
+    <t>local</t>
   </si>
 </sst>
 </file>
@@ -390,7 +399,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="24">
+  <cellStyleXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -401,6 +410,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -444,7 +455,7 @@
     <xf numFmtId="9" fontId="8" fillId="3" borderId="1" xfId="9" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="9" fillId="3" borderId="1" xfId="9" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="24">
+  <cellStyles count="26">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -456,6 +467,7 @@
     <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -467,6 +479,7 @@
     <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="9" builtinId="5"/>
   </cellStyles>
@@ -797,10 +810,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P58"/>
+  <dimension ref="A1:P61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="K42" sqref="K42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -982,7 +995,9 @@
       <c r="J6" s="11">
         <v>1</v>
       </c>
-      <c r="K6" s="11"/>
+      <c r="K6" s="11">
+        <v>1</v>
+      </c>
       <c r="L6" s="11">
         <v>1</v>
       </c>
@@ -1578,127 +1593,127 @@
     </row>
     <row r="21" spans="1:16">
       <c r="B21" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="11">
+        <v>1</v>
+      </c>
+      <c r="D21" s="11">
+        <v>0</v>
+      </c>
+      <c r="E21" s="11">
+        <v>1</v>
+      </c>
+      <c r="F21" s="11">
+        <v>1</v>
+      </c>
+      <c r="G21" s="11">
+        <v>1</v>
+      </c>
+      <c r="H21" s="11">
+        <v>1</v>
+      </c>
+      <c r="I21" s="11">
+        <v>1</v>
+      </c>
+      <c r="J21" s="11">
+        <v>1</v>
+      </c>
+      <c r="K21" s="11">
+        <v>1</v>
+      </c>
+      <c r="L21" s="11">
+        <v>1</v>
+      </c>
+      <c r="M21" s="11">
+        <v>1</v>
+      </c>
+      <c r="N21" s="11">
+        <v>1</v>
+      </c>
+      <c r="O21" s="11">
+        <v>1</v>
+      </c>
+      <c r="P21" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="B22" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C21" s="11">
-        <v>1</v>
-      </c>
-      <c r="D21" s="11">
-        <v>0</v>
-      </c>
-      <c r="E21" s="11">
-        <v>0</v>
-      </c>
-      <c r="F21" s="11">
-        <v>1</v>
-      </c>
-      <c r="G21" s="11">
-        <v>0</v>
-      </c>
-      <c r="H21" s="11">
-        <v>1</v>
-      </c>
-      <c r="I21" s="11">
-        <v>0</v>
-      </c>
-      <c r="J21" s="11">
-        <v>1</v>
-      </c>
-      <c r="K21" s="11">
-        <v>1</v>
-      </c>
-      <c r="L21" s="11">
-        <v>0</v>
-      </c>
-      <c r="M21" s="11">
-        <v>0</v>
-      </c>
-      <c r="N21" s="11">
-        <v>0</v>
-      </c>
-      <c r="O21" s="11">
-        <v>1</v>
-      </c>
-      <c r="P21" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16">
-      <c r="A22" s="2" t="s">
+      <c r="C22" s="11">
+        <v>1</v>
+      </c>
+      <c r="D22" s="11">
+        <v>0</v>
+      </c>
+      <c r="E22" s="11">
+        <v>0</v>
+      </c>
+      <c r="F22" s="11">
+        <v>1</v>
+      </c>
+      <c r="G22" s="11">
+        <v>0</v>
+      </c>
+      <c r="H22" s="11">
+        <v>1</v>
+      </c>
+      <c r="I22" s="11">
+        <v>0</v>
+      </c>
+      <c r="J22" s="11">
+        <v>1</v>
+      </c>
+      <c r="K22" s="11">
+        <v>1</v>
+      </c>
+      <c r="L22" s="11">
+        <v>0</v>
+      </c>
+      <c r="M22" s="11">
+        <v>0</v>
+      </c>
+      <c r="N22" s="11">
+        <v>0</v>
+      </c>
+      <c r="O22" s="11">
+        <v>1</v>
+      </c>
+      <c r="P22" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="A23" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="8"/>
-      <c r="N22" s="8"/>
-      <c r="O22" s="8"/>
-      <c r="P22" s="9"/>
-    </row>
-    <row r="23" spans="1:16">
-      <c r="B23" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="11">
-        <v>1</v>
-      </c>
-      <c r="D23" s="11">
-        <v>1</v>
-      </c>
-      <c r="E23" s="11">
-        <v>1</v>
-      </c>
-      <c r="F23" s="11">
-        <v>1</v>
-      </c>
-      <c r="G23" s="11">
-        <v>1</v>
-      </c>
-      <c r="H23" s="11">
-        <v>1</v>
-      </c>
-      <c r="I23" s="11">
-        <v>1</v>
-      </c>
-      <c r="J23" s="11">
-        <v>1</v>
-      </c>
-      <c r="K23" s="11">
-        <v>1</v>
-      </c>
-      <c r="L23" s="11">
-        <v>1</v>
-      </c>
-      <c r="M23" s="11">
-        <v>1</v>
-      </c>
-      <c r="N23" s="11">
-        <v>1</v>
-      </c>
-      <c r="O23" s="11">
-        <v>1</v>
-      </c>
-      <c r="P23" s="11">
-        <v>1</v>
-      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="9"/>
     </row>
     <row r="24" spans="1:16">
       <c r="B24" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C24" s="11">
         <v>1</v>
       </c>
       <c r="D24" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" s="11">
         <v>1</v>
@@ -1739,124 +1754,124 @@
     </row>
     <row r="25" spans="1:16">
       <c r="B25" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="11">
+        <v>1</v>
+      </c>
+      <c r="D25" s="11">
+        <v>0</v>
+      </c>
+      <c r="E25" s="11">
+        <v>1</v>
+      </c>
+      <c r="F25" s="11">
+        <v>1</v>
+      </c>
+      <c r="G25" s="11">
+        <v>1</v>
+      </c>
+      <c r="H25" s="11">
+        <v>1</v>
+      </c>
+      <c r="I25" s="11">
+        <v>1</v>
+      </c>
+      <c r="J25" s="11">
+        <v>1</v>
+      </c>
+      <c r="K25" s="11">
+        <v>1</v>
+      </c>
+      <c r="L25" s="11">
+        <v>1</v>
+      </c>
+      <c r="M25" s="11">
+        <v>1</v>
+      </c>
+      <c r="N25" s="11">
+        <v>1</v>
+      </c>
+      <c r="O25" s="11">
+        <v>1</v>
+      </c>
+      <c r="P25" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
+      <c r="B26" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C25" s="11">
-        <v>0</v>
-      </c>
-      <c r="D25" s="11">
-        <v>1</v>
-      </c>
-      <c r="E25" s="11">
-        <v>1</v>
-      </c>
-      <c r="F25" s="11">
-        <v>1</v>
-      </c>
-      <c r="G25" s="11">
-        <v>1</v>
-      </c>
-      <c r="H25" s="11">
-        <v>1</v>
-      </c>
-      <c r="I25" s="11">
-        <v>0</v>
-      </c>
-      <c r="J25" s="11">
-        <v>1</v>
-      </c>
-      <c r="K25" s="11">
-        <v>1</v>
-      </c>
-      <c r="L25" s="11">
-        <v>1</v>
-      </c>
-      <c r="M25" s="11">
-        <v>1</v>
-      </c>
-      <c r="N25" s="11">
-        <v>1</v>
-      </c>
-      <c r="O25" s="11">
-        <v>1</v>
-      </c>
-      <c r="P25" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16">
-      <c r="A26" s="2" t="s">
+      <c r="C26" s="11">
+        <v>0</v>
+      </c>
+      <c r="D26" s="11">
+        <v>1</v>
+      </c>
+      <c r="E26" s="11">
+        <v>1</v>
+      </c>
+      <c r="F26" s="11">
+        <v>1</v>
+      </c>
+      <c r="G26" s="11">
+        <v>1</v>
+      </c>
+      <c r="H26" s="11">
+        <v>1</v>
+      </c>
+      <c r="I26" s="11">
+        <v>0</v>
+      </c>
+      <c r="J26" s="11">
+        <v>1</v>
+      </c>
+      <c r="K26" s="11">
+        <v>1</v>
+      </c>
+      <c r="L26" s="11">
+        <v>1</v>
+      </c>
+      <c r="M26" s="11">
+        <v>1</v>
+      </c>
+      <c r="N26" s="11">
+        <v>1</v>
+      </c>
+      <c r="O26" s="11">
+        <v>1</v>
+      </c>
+      <c r="P26" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
+      <c r="A27" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
-      <c r="L26" s="8"/>
-      <c r="M26" s="8"/>
-      <c r="N26" s="8"/>
-      <c r="O26" s="8"/>
-      <c r="P26" s="9"/>
-    </row>
-    <row r="27" spans="1:16">
-      <c r="B27" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C27" s="11">
-        <v>1</v>
-      </c>
-      <c r="D27" s="11">
-        <v>0</v>
-      </c>
-      <c r="E27" s="11">
-        <v>0</v>
-      </c>
-      <c r="F27" s="11">
-        <v>1</v>
-      </c>
-      <c r="G27" s="11">
-        <v>0</v>
-      </c>
-      <c r="H27" s="11">
-        <v>1</v>
-      </c>
-      <c r="I27" s="11">
-        <v>1</v>
-      </c>
-      <c r="J27" s="11">
-        <v>1</v>
-      </c>
-      <c r="K27" s="11">
-        <v>1</v>
-      </c>
-      <c r="L27" s="11">
-        <v>1</v>
-      </c>
-      <c r="M27" s="11">
-        <v>1</v>
-      </c>
-      <c r="N27" s="11">
-        <v>1</v>
-      </c>
-      <c r="O27" s="11">
-        <v>1</v>
-      </c>
-      <c r="P27" s="11">
-        <v>1</v>
-      </c>
+      <c r="B27" s="4"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="8"/>
+      <c r="P27" s="9"/>
     </row>
     <row r="28" spans="1:16">
       <c r="B28" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C28" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D28" s="11">
         <v>0</v>
@@ -1868,7 +1883,7 @@
         <v>1</v>
       </c>
       <c r="G28" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H28" s="11">
         <v>1</v>
@@ -1900,7 +1915,7 @@
     </row>
     <row r="29" spans="1:16">
       <c r="B29" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C29" s="11">
         <v>0</v>
@@ -1947,7 +1962,7 @@
     </row>
     <row r="30" spans="1:16">
       <c r="B30" s="6" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="C30" s="11">
         <v>0</v>
@@ -1968,13 +1983,13 @@
         <v>1</v>
       </c>
       <c r="I30" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J30" s="11">
         <v>1</v>
       </c>
       <c r="K30" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L30" s="11">
         <v>1</v>
@@ -1983,135 +1998,135 @@
         <v>1</v>
       </c>
       <c r="N30" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O30" s="11">
         <v>1</v>
       </c>
       <c r="P30" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:16">
       <c r="B31" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" s="11">
+        <v>0</v>
+      </c>
+      <c r="D31" s="11">
+        <v>0</v>
+      </c>
+      <c r="E31" s="11">
+        <v>0</v>
+      </c>
+      <c r="F31" s="11">
+        <v>1</v>
+      </c>
+      <c r="G31" s="11">
+        <v>1</v>
+      </c>
+      <c r="H31" s="11">
+        <v>1</v>
+      </c>
+      <c r="I31" s="11">
+        <v>0</v>
+      </c>
+      <c r="J31" s="11">
+        <v>1</v>
+      </c>
+      <c r="K31" s="11">
+        <v>1</v>
+      </c>
+      <c r="L31" s="11">
+        <v>1</v>
+      </c>
+      <c r="M31" s="11">
+        <v>1</v>
+      </c>
+      <c r="N31" s="11">
+        <v>0</v>
+      </c>
+      <c r="O31" s="11">
+        <v>1</v>
+      </c>
+      <c r="P31" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
+      <c r="B32" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="11">
-        <v>0</v>
-      </c>
-      <c r="D31" s="11">
-        <v>0</v>
-      </c>
-      <c r="E31" s="11">
-        <v>0</v>
-      </c>
-      <c r="F31" s="11">
-        <v>1</v>
-      </c>
-      <c r="G31" s="11">
-        <v>1</v>
-      </c>
-      <c r="H31" s="11">
-        <v>1</v>
-      </c>
-      <c r="I31" s="11">
-        <v>0</v>
-      </c>
-      <c r="J31" s="11">
-        <v>1</v>
-      </c>
-      <c r="K31" s="11">
-        <v>1</v>
-      </c>
-      <c r="L31" s="11">
-        <v>1</v>
-      </c>
-      <c r="M31" s="11">
-        <v>1</v>
-      </c>
-      <c r="N31" s="11">
-        <v>1</v>
-      </c>
-      <c r="O31" s="11">
-        <v>1</v>
-      </c>
-      <c r="P31" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16">
-      <c r="A32" s="2" t="s">
+      <c r="C32" s="11">
+        <v>0</v>
+      </c>
+      <c r="D32" s="11">
+        <v>0</v>
+      </c>
+      <c r="E32" s="11">
+        <v>0</v>
+      </c>
+      <c r="F32" s="11">
+        <v>1</v>
+      </c>
+      <c r="G32" s="11">
+        <v>1</v>
+      </c>
+      <c r="H32" s="11">
+        <v>1</v>
+      </c>
+      <c r="I32" s="11">
+        <v>0</v>
+      </c>
+      <c r="J32" s="11">
+        <v>1</v>
+      </c>
+      <c r="K32" s="11">
+        <v>1</v>
+      </c>
+      <c r="L32" s="11">
+        <v>1</v>
+      </c>
+      <c r="M32" s="11">
+        <v>1</v>
+      </c>
+      <c r="N32" s="11">
+        <v>1</v>
+      </c>
+      <c r="O32" s="11">
+        <v>1</v>
+      </c>
+      <c r="P32" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
+      <c r="A33" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="4"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
-      <c r="K32" s="8"/>
-      <c r="L32" s="8"/>
-      <c r="M32" s="8"/>
-      <c r="N32" s="8"/>
-      <c r="O32" s="8"/>
-      <c r="P32" s="9"/>
-    </row>
-    <row r="33" spans="1:16">
-      <c r="B33" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C33" s="11">
-        <v>1</v>
-      </c>
-      <c r="D33" s="11">
-        <v>0</v>
-      </c>
-      <c r="E33" s="11">
-        <v>0</v>
-      </c>
-      <c r="F33" s="11">
-        <v>0</v>
-      </c>
-      <c r="G33" s="11">
-        <v>0</v>
-      </c>
-      <c r="H33" s="11">
-        <v>1</v>
-      </c>
-      <c r="I33" s="11">
-        <v>1</v>
-      </c>
-      <c r="J33" s="11">
-        <v>1</v>
-      </c>
-      <c r="K33" s="11">
-        <v>1</v>
-      </c>
-      <c r="L33" s="11">
-        <v>1</v>
-      </c>
-      <c r="M33" s="11">
-        <v>1</v>
-      </c>
-      <c r="N33" s="11">
-        <v>1</v>
-      </c>
-      <c r="O33" s="11">
-        <v>1</v>
-      </c>
-      <c r="P33" s="11">
-        <v>0</v>
-      </c>
+      <c r="B33" s="4"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8"/>
+      <c r="K33" s="8"/>
+      <c r="L33" s="8"/>
+      <c r="M33" s="8"/>
+      <c r="N33" s="8"/>
+      <c r="O33" s="8"/>
+      <c r="P33" s="9"/>
     </row>
     <row r="34" spans="1:16">
       <c r="B34" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C34" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D34" s="11">
         <v>0</v>
@@ -2155,7 +2170,7 @@
     </row>
     <row r="35" spans="1:16">
       <c r="B35" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C35" s="11">
         <v>0</v>
@@ -2176,7 +2191,7 @@
         <v>1</v>
       </c>
       <c r="I35" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J35" s="11">
         <v>1</v>
@@ -2202,7 +2217,7 @@
     </row>
     <row r="36" spans="1:16">
       <c r="B36" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C36" s="11">
         <v>0</v>
@@ -2241,7 +2256,7 @@
         <v>1</v>
       </c>
       <c r="O36" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P36" s="11">
         <v>0</v>
@@ -2249,282 +2264,287 @@
     </row>
     <row r="37" spans="1:16">
       <c r="B37" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C37" s="11">
+        <v>0</v>
+      </c>
+      <c r="D37" s="11">
+        <v>0</v>
+      </c>
+      <c r="E37" s="11">
+        <v>0</v>
+      </c>
+      <c r="F37" s="11">
+        <v>0</v>
+      </c>
+      <c r="G37" s="11">
+        <v>0</v>
+      </c>
+      <c r="H37" s="11">
+        <v>1</v>
+      </c>
+      <c r="I37" s="11">
+        <v>0</v>
+      </c>
+      <c r="J37" s="11">
+        <v>1</v>
+      </c>
+      <c r="K37" s="11">
+        <v>1</v>
+      </c>
+      <c r="L37" s="11">
+        <v>1</v>
+      </c>
+      <c r="M37" s="11">
+        <v>1</v>
+      </c>
+      <c r="N37" s="11">
+        <v>1</v>
+      </c>
+      <c r="O37" s="11">
+        <v>0</v>
+      </c>
+      <c r="P37" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16">
+      <c r="B38" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C37" s="11">
-        <v>0</v>
-      </c>
-      <c r="D37" s="11">
-        <v>0</v>
-      </c>
-      <c r="E37" s="11">
-        <v>0</v>
-      </c>
-      <c r="F37" s="11">
-        <v>0</v>
-      </c>
-      <c r="G37" s="11">
-        <v>0</v>
-      </c>
-      <c r="H37" s="11">
-        <v>1</v>
-      </c>
-      <c r="I37" s="11">
-        <v>0</v>
-      </c>
-      <c r="J37" s="11">
-        <v>1</v>
-      </c>
-      <c r="K37" s="11">
-        <v>1</v>
-      </c>
-      <c r="L37" s="11">
-        <v>1</v>
-      </c>
-      <c r="M37" s="11">
-        <v>1</v>
-      </c>
-      <c r="N37" s="11">
-        <v>1</v>
-      </c>
-      <c r="O37" s="11">
-        <v>1</v>
-      </c>
-      <c r="P37" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16">
-      <c r="A38" s="2" t="s">
+      <c r="C38" s="11">
+        <v>0</v>
+      </c>
+      <c r="D38" s="11">
+        <v>0</v>
+      </c>
+      <c r="E38" s="11">
+        <v>0</v>
+      </c>
+      <c r="F38" s="11">
+        <v>0</v>
+      </c>
+      <c r="G38" s="11">
+        <v>0</v>
+      </c>
+      <c r="H38" s="11">
+        <v>1</v>
+      </c>
+      <c r="I38" s="11">
+        <v>0</v>
+      </c>
+      <c r="J38" s="11">
+        <v>1</v>
+      </c>
+      <c r="K38" s="11">
+        <v>1</v>
+      </c>
+      <c r="L38" s="11">
+        <v>1</v>
+      </c>
+      <c r="M38" s="11">
+        <v>1</v>
+      </c>
+      <c r="N38" s="11">
+        <v>1</v>
+      </c>
+      <c r="O38" s="11">
+        <v>1</v>
+      </c>
+      <c r="P38" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16">
+      <c r="A39" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B38" s="4"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
-      <c r="J38" s="8"/>
-      <c r="K38" s="8"/>
-      <c r="L38" s="8"/>
-      <c r="M38" s="8"/>
-      <c r="N38" s="8"/>
-      <c r="O38" s="8"/>
-      <c r="P38" s="9"/>
-    </row>
-    <row r="39" spans="1:16">
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="4"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
+      <c r="K39" s="8"/>
+      <c r="L39" s="8"/>
+      <c r="M39" s="8"/>
+      <c r="N39" s="8"/>
+      <c r="O39" s="8"/>
+      <c r="P39" s="9"/>
+    </row>
+    <row r="40" spans="1:16">
+      <c r="B40" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C39" s="11">
-        <v>1</v>
-      </c>
-      <c r="D39" s="11">
-        <v>0</v>
-      </c>
-      <c r="E39" s="11">
-        <v>1</v>
-      </c>
-      <c r="F39" s="11"/>
-      <c r="G39" s="11">
-        <v>0</v>
-      </c>
-      <c r="H39" s="11"/>
-      <c r="I39" s="11">
-        <v>1</v>
-      </c>
-      <c r="J39" s="11"/>
-      <c r="K39" s="11"/>
-      <c r="L39" s="11">
-        <v>1</v>
-      </c>
-      <c r="M39" s="11">
-        <v>1</v>
-      </c>
-      <c r="N39" s="11">
-        <v>1</v>
-      </c>
-      <c r="O39" s="11"/>
-      <c r="P39" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16">
-      <c r="A40" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B40" s="4"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8"/>
-      <c r="I40" s="8"/>
-      <c r="J40" s="8"/>
-      <c r="K40" s="8"/>
-      <c r="L40" s="8"/>
-      <c r="M40" s="8"/>
-      <c r="N40" s="8"/>
-      <c r="O40" s="8"/>
-      <c r="P40" s="9"/>
+      <c r="C40" s="11">
+        <v>1</v>
+      </c>
+      <c r="D40" s="11">
+        <v>0</v>
+      </c>
+      <c r="E40" s="11">
+        <v>1</v>
+      </c>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11">
+        <v>0</v>
+      </c>
+      <c r="H40" s="11"/>
+      <c r="I40" s="11">
+        <v>1</v>
+      </c>
+      <c r="J40" s="11"/>
+      <c r="K40" s="11">
+        <v>1</v>
+      </c>
+      <c r="L40" s="11">
+        <v>1</v>
+      </c>
+      <c r="M40" s="11">
+        <v>1</v>
+      </c>
+      <c r="N40" s="11">
+        <v>1</v>
+      </c>
+      <c r="O40" s="11"/>
+      <c r="P40" s="11">
+        <v>1</v>
+      </c>
     </row>
     <row r="41" spans="1:16">
       <c r="B41" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C41" s="11">
-        <v>1</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="C41" s="11"/>
       <c r="D41" s="11">
         <v>0</v>
       </c>
-      <c r="E41" s="11">
-        <v>1</v>
-      </c>
+      <c r="E41" s="11"/>
       <c r="F41" s="11"/>
       <c r="G41" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H41" s="11"/>
-      <c r="I41" s="11">
-        <v>1</v>
-      </c>
+      <c r="I41" s="11"/>
       <c r="J41" s="11"/>
       <c r="K41" s="11"/>
-      <c r="L41" s="11">
-        <v>1</v>
-      </c>
-      <c r="M41" s="11">
-        <v>1</v>
-      </c>
-      <c r="N41" s="11">
-        <v>1</v>
-      </c>
+      <c r="L41" s="11"/>
+      <c r="M41" s="11"/>
+      <c r="N41" s="11"/>
       <c r="O41" s="11"/>
-      <c r="P41" s="11">
-        <v>1</v>
-      </c>
+      <c r="P41" s="11"/>
     </row>
     <row r="42" spans="1:16">
       <c r="B42" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C42" s="11">
-        <v>0</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="C42" s="11"/>
       <c r="D42" s="11">
-        <v>1</v>
-      </c>
-      <c r="E42" s="11">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E42" s="11"/>
       <c r="F42" s="11"/>
       <c r="G42" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H42" s="11"/>
-      <c r="I42" s="11">
-        <v>1</v>
-      </c>
+      <c r="I42" s="11"/>
       <c r="J42" s="11"/>
       <c r="K42" s="11"/>
-      <c r="L42" s="11">
-        <v>1</v>
-      </c>
-      <c r="M42" s="11">
-        <v>1</v>
-      </c>
-      <c r="N42" s="11">
-        <v>1</v>
-      </c>
+      <c r="L42" s="11"/>
+      <c r="M42" s="11"/>
+      <c r="N42" s="11"/>
       <c r="O42" s="11"/>
-      <c r="P42" s="11">
-        <v>1</v>
-      </c>
+      <c r="P42" s="11"/>
     </row>
     <row r="43" spans="1:16">
-      <c r="B43" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C43" s="11">
-        <v>1</v>
-      </c>
-      <c r="D43" s="11">
-        <v>1</v>
-      </c>
-      <c r="E43" s="11">
-        <v>1</v>
-      </c>
-      <c r="F43" s="11"/>
-      <c r="G43" s="11">
-        <v>1</v>
-      </c>
-      <c r="H43" s="11"/>
-      <c r="I43" s="11">
-        <v>1</v>
-      </c>
-      <c r="J43" s="11"/>
-      <c r="K43" s="11"/>
-      <c r="L43" s="11">
-        <v>1</v>
-      </c>
-      <c r="M43" s="11">
-        <v>1</v>
-      </c>
-      <c r="N43" s="11">
-        <v>1</v>
-      </c>
-      <c r="O43" s="11"/>
-      <c r="P43" s="11">
-        <v>1</v>
-      </c>
+      <c r="A43" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B43" s="4"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8"/>
+      <c r="J43" s="8"/>
+      <c r="K43" s="8"/>
+      <c r="L43" s="8"/>
+      <c r="M43" s="8"/>
+      <c r="N43" s="8"/>
+      <c r="O43" s="8"/>
+      <c r="P43" s="9"/>
     </row>
     <row r="44" spans="1:16">
-      <c r="A44" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B44" s="4"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="8"/>
-      <c r="E44" s="8"/>
-      <c r="F44" s="8"/>
-      <c r="G44" s="8"/>
-      <c r="H44" s="8"/>
-      <c r="I44" s="8"/>
-      <c r="J44" s="8"/>
-      <c r="K44" s="8"/>
-      <c r="L44" s="8"/>
-      <c r="M44" s="8"/>
-      <c r="N44" s="8"/>
-      <c r="O44" s="8"/>
-      <c r="P44" s="9"/>
+      <c r="B44" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C44" s="11">
+        <v>1</v>
+      </c>
+      <c r="D44" s="11">
+        <v>0</v>
+      </c>
+      <c r="E44" s="11">
+        <v>1</v>
+      </c>
+      <c r="F44" s="11"/>
+      <c r="G44" s="11">
+        <v>1</v>
+      </c>
+      <c r="H44" s="11"/>
+      <c r="I44" s="11">
+        <v>1</v>
+      </c>
+      <c r="J44" s="11"/>
+      <c r="K44" s="11">
+        <v>1</v>
+      </c>
+      <c r="L44" s="11">
+        <v>1</v>
+      </c>
+      <c r="M44" s="11">
+        <v>1</v>
+      </c>
+      <c r="N44" s="11">
+        <v>1</v>
+      </c>
+      <c r="O44" s="11"/>
+      <c r="P44" s="11">
+        <v>1</v>
+      </c>
     </row>
     <row r="45" spans="1:16">
       <c r="B45" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C45" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D45" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E45" s="11">
         <v>1</v>
       </c>
       <c r="F45" s="11"/>
       <c r="G45" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H45" s="11"/>
       <c r="I45" s="11">
         <v>1</v>
       </c>
       <c r="J45" s="11"/>
-      <c r="K45" s="11"/>
+      <c r="K45" s="11">
+        <v>1</v>
+      </c>
       <c r="L45" s="11">
         <v>1</v>
       </c>
@@ -2541,27 +2561,29 @@
     </row>
     <row r="46" spans="1:16">
       <c r="B46" s="6" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="C46" s="11">
         <v>1</v>
       </c>
       <c r="D46" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E46" s="11">
         <v>1</v>
       </c>
       <c r="F46" s="11"/>
       <c r="G46" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H46" s="11"/>
       <c r="I46" s="11">
         <v>1</v>
       </c>
       <c r="J46" s="11"/>
-      <c r="K46" s="11"/>
+      <c r="K46" s="11">
+        <v>1</v>
+      </c>
       <c r="L46" s="11">
         <v>1</v>
       </c>
@@ -2577,65 +2599,67 @@
       </c>
     </row>
     <row r="47" spans="1:16">
-      <c r="B47" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C47" s="11">
-        <v>0</v>
-      </c>
-      <c r="D47" s="11">
-        <v>0</v>
-      </c>
-      <c r="E47" s="11">
-        <v>1</v>
-      </c>
-      <c r="F47" s="11"/>
-      <c r="G47" s="11">
-        <v>0</v>
-      </c>
-      <c r="H47" s="11"/>
-      <c r="I47" s="11">
-        <v>0</v>
-      </c>
-      <c r="J47" s="11"/>
-      <c r="K47" s="11"/>
-      <c r="L47" s="11">
-        <v>1</v>
-      </c>
-      <c r="M47" s="11">
-        <v>1</v>
-      </c>
-      <c r="N47" s="11">
-        <v>1</v>
-      </c>
-      <c r="O47" s="11"/>
-      <c r="P47" s="11">
-        <v>0</v>
-      </c>
+      <c r="A47" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B47" s="4"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="8"/>
+      <c r="H47" s="8"/>
+      <c r="I47" s="8"/>
+      <c r="J47" s="8"/>
+      <c r="K47" s="8"/>
+      <c r="L47" s="8"/>
+      <c r="M47" s="8"/>
+      <c r="N47" s="8"/>
+      <c r="O47" s="8"/>
+      <c r="P47" s="9"/>
     </row>
     <row r="48" spans="1:16">
-      <c r="A48" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B48" s="4"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="8"/>
-      <c r="E48" s="8"/>
-      <c r="F48" s="8"/>
-      <c r="G48" s="8"/>
-      <c r="H48" s="8"/>
-      <c r="I48" s="8"/>
-      <c r="J48" s="8"/>
-      <c r="K48" s="8"/>
-      <c r="L48" s="8"/>
-      <c r="M48" s="8"/>
-      <c r="N48" s="8"/>
-      <c r="O48" s="8"/>
-      <c r="P48" s="9"/>
-    </row>
-    <row r="49" spans="2:16">
+      <c r="B48" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C48" s="11">
+        <v>1</v>
+      </c>
+      <c r="D48" s="11">
+        <v>0</v>
+      </c>
+      <c r="E48" s="11">
+        <v>1</v>
+      </c>
+      <c r="F48" s="11"/>
+      <c r="G48" s="11">
+        <v>0</v>
+      </c>
+      <c r="H48" s="11"/>
+      <c r="I48" s="11">
+        <v>1</v>
+      </c>
+      <c r="J48" s="11"/>
+      <c r="K48" s="11">
+        <v>1</v>
+      </c>
+      <c r="L48" s="11">
+        <v>1</v>
+      </c>
+      <c r="M48" s="11">
+        <v>1</v>
+      </c>
+      <c r="N48" s="11">
+        <v>1</v>
+      </c>
+      <c r="O48" s="11"/>
+      <c r="P48" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16">
       <c r="B49" s="6" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C49" s="11">
         <v>1</v>
@@ -2644,7 +2668,7 @@
         <v>0</v>
       </c>
       <c r="E49" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F49" s="11"/>
       <c r="G49" s="11">
@@ -2655,7 +2679,9 @@
         <v>1</v>
       </c>
       <c r="J49" s="11"/>
-      <c r="K49" s="11"/>
+      <c r="K49" s="11">
+        <v>1</v>
+      </c>
       <c r="L49" s="11">
         <v>1</v>
       </c>
@@ -2670,18 +2696,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="2:16">
+    <row r="50" spans="1:16">
       <c r="B50" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C50" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D50" s="11">
         <v>0</v>
       </c>
       <c r="E50" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F50" s="11"/>
       <c r="G50" s="11">
@@ -2689,10 +2715,12 @@
       </c>
       <c r="H50" s="11"/>
       <c r="I50" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J50" s="11"/>
-      <c r="K50" s="11"/>
+      <c r="K50" s="11">
+        <v>1</v>
+      </c>
       <c r="L50" s="11">
         <v>1</v>
       </c>
@@ -2704,105 +2732,205 @@
       </c>
       <c r="O50" s="11"/>
       <c r="P50" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="2:16">
-      <c r="B51" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16">
+      <c r="A51" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B51" s="4"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="8"/>
+      <c r="E51" s="8"/>
+      <c r="F51" s="8"/>
+      <c r="G51" s="8"/>
+      <c r="H51" s="8"/>
+      <c r="I51" s="8"/>
+      <c r="J51" s="8"/>
+      <c r="K51" s="8"/>
+      <c r="L51" s="8"/>
+      <c r="M51" s="8"/>
+      <c r="N51" s="8"/>
+      <c r="O51" s="8"/>
+      <c r="P51" s="9"/>
+    </row>
+    <row r="52" spans="1:16">
+      <c r="B52" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C52" s="11">
+        <v>1</v>
+      </c>
+      <c r="D52" s="11">
+        <v>0</v>
+      </c>
+      <c r="E52" s="11">
+        <v>0</v>
+      </c>
+      <c r="F52" s="11"/>
+      <c r="G52" s="11">
+        <v>0</v>
+      </c>
+      <c r="H52" s="11"/>
+      <c r="I52" s="11">
+        <v>1</v>
+      </c>
+      <c r="J52" s="11"/>
+      <c r="K52" s="11">
+        <v>1</v>
+      </c>
+      <c r="L52" s="11">
+        <v>1</v>
+      </c>
+      <c r="M52" s="11">
+        <v>1</v>
+      </c>
+      <c r="N52" s="11">
+        <v>1</v>
+      </c>
+      <c r="O52" s="11"/>
+      <c r="P52" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16">
+      <c r="B53" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C53" s="11">
+        <v>1</v>
+      </c>
+      <c r="D53" s="11">
+        <v>0</v>
+      </c>
+      <c r="E53" s="11">
+        <v>0</v>
+      </c>
+      <c r="F53" s="11"/>
+      <c r="G53" s="11">
+        <v>0</v>
+      </c>
+      <c r="H53" s="11"/>
+      <c r="I53" s="11">
+        <v>1</v>
+      </c>
+      <c r="J53" s="11"/>
+      <c r="K53" s="11">
+        <v>1</v>
+      </c>
+      <c r="L53" s="11">
+        <v>1</v>
+      </c>
+      <c r="M53" s="11">
+        <v>1</v>
+      </c>
+      <c r="N53" s="11">
+        <v>1</v>
+      </c>
+      <c r="O53" s="11"/>
+      <c r="P53" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16">
+      <c r="B54" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C51" s="11">
-        <v>0</v>
-      </c>
-      <c r="D51" s="11">
-        <v>0</v>
-      </c>
-      <c r="E51" s="11">
-        <v>0</v>
-      </c>
-      <c r="F51" s="11"/>
-      <c r="G51" s="11">
-        <v>0</v>
-      </c>
-      <c r="H51" s="11"/>
-      <c r="I51" s="11"/>
-      <c r="J51" s="11"/>
-      <c r="K51" s="11"/>
-      <c r="L51" s="11"/>
-      <c r="M51" s="11"/>
-      <c r="N51" s="11"/>
-      <c r="O51" s="11"/>
-      <c r="P51" s="11"/>
-    </row>
-    <row r="53" spans="2:16">
-      <c r="B53" s="6" t="s">
+      <c r="C54" s="11">
+        <v>0</v>
+      </c>
+      <c r="D54" s="11">
+        <v>0</v>
+      </c>
+      <c r="E54" s="11">
+        <v>0</v>
+      </c>
+      <c r="F54" s="11"/>
+      <c r="G54" s="11">
+        <v>0</v>
+      </c>
+      <c r="H54" s="11"/>
+      <c r="I54" s="11"/>
+      <c r="J54" s="11"/>
+      <c r="K54" s="11">
+        <v>1</v>
+      </c>
+      <c r="L54" s="11"/>
+      <c r="M54" s="11"/>
+      <c r="N54" s="11"/>
+      <c r="O54" s="11"/>
+      <c r="P54" s="11"/>
+    </row>
+    <row r="56" spans="1:16">
+      <c r="B56" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C53" s="13">
-        <f>SUM(C3:C50)/COUNT(C3:C50)</f>
-        <v>0.63888888888888884</v>
-      </c>
-      <c r="D53" s="12">
-        <f t="shared" ref="D53:P53" si="0">SUM(D3:D51)/COUNT(D3:D51)</f>
-        <v>0.27027027027027029</v>
-      </c>
-      <c r="E53" s="12">
+      <c r="C56" s="13">
+        <f>SUM(C3:C53)/COUNT(C3:C53)</f>
+        <v>0.64864864864864868</v>
+      </c>
+      <c r="D56" s="12">
+        <f t="shared" ref="D56:P56" si="0">SUM(D3:D54)/COUNT(D3:D54)</f>
+        <v>0.25</v>
+      </c>
+      <c r="E56" s="12">
         <f t="shared" si="0"/>
-        <v>0.59459459459459463</v>
-      </c>
-      <c r="F53" s="12">
+        <v>0.60526315789473684</v>
+      </c>
+      <c r="F56" s="12">
         <f t="shared" si="0"/>
-        <v>0.80769230769230771</v>
-      </c>
-      <c r="G53" s="12">
+        <v>0.81481481481481477</v>
+      </c>
+      <c r="G56" s="12">
         <f t="shared" si="0"/>
-        <v>0.54054054054054057</v>
-      </c>
-      <c r="H53" s="12">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="H56" s="12">
         <f t="shared" si="0"/>
-        <v>0.96296296296296291</v>
-      </c>
-      <c r="I53" s="12">
+        <v>0.9642857142857143</v>
+      </c>
+      <c r="I56" s="12">
         <f t="shared" si="0"/>
-        <v>0.72222222222222221</v>
-      </c>
-      <c r="J53" s="12">
+        <v>0.72972972972972971</v>
+      </c>
+      <c r="J56" s="12">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K53" s="12">
+      <c r="K56" s="12">
         <f t="shared" si="0"/>
-        <v>0.92307692307692313</v>
-      </c>
-      <c r="L53" s="12">
+        <v>0.97368421052631582</v>
+      </c>
+      <c r="L56" s="12">
         <f t="shared" si="0"/>
-        <v>0.97222222222222221</v>
-      </c>
-      <c r="M53" s="12">
+        <v>0.97297297297297303</v>
+      </c>
+      <c r="M56" s="12">
         <f t="shared" si="0"/>
-        <v>0.91666666666666663</v>
-      </c>
-      <c r="N53" s="12">
+        <v>0.91891891891891897</v>
+      </c>
+      <c r="N56" s="12">
         <f t="shared" si="0"/>
-        <v>0.94444444444444442</v>
-      </c>
-      <c r="O53" s="12">
+        <v>0.94594594594594594</v>
+      </c>
+      <c r="O56" s="12">
         <f t="shared" si="0"/>
-        <v>0.92592592592592593</v>
-      </c>
-      <c r="P53" s="12">
+        <v>0.9285714285714286</v>
+      </c>
+      <c r="P56" s="12">
         <f t="shared" si="0"/>
-        <v>0.72222222222222221</v>
-      </c>
-    </row>
-    <row r="56" spans="2:16">
-      <c r="B56"/>
-    </row>
-    <row r="57" spans="2:16">
-      <c r="B57"/>
-    </row>
-    <row r="58" spans="2:16">
-      <c r="B58"/>
+        <v>0.72972972972972971</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16">
+      <c r="B59"/>
+    </row>
+    <row r="60" spans="1:16">
+      <c r="B60"/>
+    </row>
+    <row r="61" spans="1:16">
+      <c r="B61"/>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>

</xml_diff>